<commit_message>
Actualización registro horas y seguimiento proyecto, V 6.0
</commit_message>
<xml_diff>
--- a/Documentacion/Fase de elaboracion/Semana 6/Gestion de proyecto/GPRACG2.xlsx
+++ b/Documentacion/Fase de elaboracion/Semana 6/Gestion de proyecto/GPRACG2.xlsx
@@ -26,13 +26,14 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId17"/>
+    <externalReference r:id="rId18"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="187">
   <si>
     <t>Javier Madeiro</t>
   </si>
@@ -382,15 +383,9 @@
     <t>Reunión para especificar casos de uso pre reunión con docente, luego reunión para estimar esfuerzo.</t>
   </si>
   <si>
-    <t>15/09/2010</t>
-  </si>
-  <si>
     <t>Corrección de errores en servicios</t>
   </si>
   <si>
-    <t>16/09/2010</t>
-  </si>
-  <si>
     <t>Reunión con Diegoy Martín para planificar y dividir el desarrollo de la semana</t>
   </si>
   <si>
@@ -563,6 +558,42 @@
   </si>
   <si>
     <t>Terminar de emprolijar el código y la estructura en el repo. Se subió lo correspondiente al WP</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Revisar entregas, informe semanal, planificar semana 6</t>
+  </si>
+  <si>
+    <t>Revisión entregas, realizar informe semanal de SQA, planificar semana</t>
+  </si>
+  <si>
+    <t>Reunión con el director</t>
+  </si>
+  <si>
+    <t>Reunión director</t>
+  </si>
+  <si>
+    <t>Revisión de entregas</t>
+  </si>
+  <si>
+    <t>Revisión de entregas, seguimiento del doc Modelo de Casos de Uso contra revisión</t>
+  </si>
+  <si>
+    <t>Estudio</t>
+  </si>
+  <si>
+    <t>Dejando las animaciones de pantalla de viajar para que se reciba lo retornado de las operaciones que se trae de Azure.</t>
+  </si>
+  <si>
+    <t>Reunión para determinar los pasos a seguir y priorizar los casos de uso. Se realizaron pruebas, analizaron variantes para las pantallas, etc.</t>
+  </si>
+  <si>
+    <t>Implementacion</t>
+  </si>
+  <si>
+    <t>Implementacion de botones de pantalla general + busqueda de imagenes a utilizar + edicion de dichas imagenes</t>
   </si>
 </sst>
 </file>
@@ -930,7 +961,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$28</c:f>
+              <c:f>[2]Hoja1!$B$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -941,7 +972,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$29:$A$41</c:f>
+              <c:f>[2]Hoja1!$A$29:$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
@@ -985,7 +1016,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$29:$B$41</c:f>
+              <c:f>[2]Hoja1!$B$29:$B$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1034,7 +1065,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$C$28</c:f>
+              <c:f>[2]Hoja1!$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1045,7 +1076,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$29:$A$41</c:f>
+              <c:f>[2]Hoja1!$A$29:$A$41</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
@@ -1089,7 +1120,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$C$29:$C$41</c:f>
+              <c:f>[2]Hoja1!$C$29:$C$41</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1109,7 +1140,7 @@
                   <c:v>14.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>14.5</c:v>
@@ -1134,24 +1165,24 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="129074304"/>
-        <c:axId val="129075840"/>
+        <c:axId val="84846848"/>
+        <c:axId val="85016576"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="129074304"/>
+        <c:axId val="84846848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129075840"/>
+        <c:crossAx val="85016576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="129075840"/>
+        <c:axId val="85016576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1159,7 +1190,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="129074304"/>
+        <c:crossAx val="84846848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1182,7 +1213,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000133" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000133" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1202,7 +1233,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$43</c:f>
+              <c:f>[2]Hoja1!$B$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1213,7 +1244,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$44:$A$56</c:f>
+              <c:f>[2]Hoja1!$A$44:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
@@ -1257,7 +1288,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$44:$B$56</c:f>
+              <c:f>[2]Hoja1!$B$44:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1306,7 +1337,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$C$43</c:f>
+              <c:f>[2]Hoja1!$C$43</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1317,7 +1348,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$44:$A$56</c:f>
+              <c:f>[2]Hoja1!$A$44:$A$56</c:f>
               <c:strCache>
                 <c:ptCount val="13"/>
                 <c:pt idx="1">
@@ -1361,7 +1392,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$C$44:$C$56</c:f>
+              <c:f>[2]Hoja1!$C$44:$C$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -1381,7 +1412,7 @@
                   <c:v>120.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>107</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>102</c:v>
@@ -1406,24 +1437,24 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="154609536"/>
-        <c:axId val="154611072"/>
+        <c:axId val="91272704"/>
+        <c:axId val="91274240"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154609536"/>
+        <c:axId val="91272704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154611072"/>
+        <c:crossAx val="91274240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154611072"/>
+        <c:axId val="91274240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1431,7 +1462,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154609536"/>
+        <c:crossAx val="91272704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1454,7 +1485,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000155" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000155" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1477,7 +1508,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$58</c:f>
+              <c:f>[2]Hoja1!$B$58</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1488,7 +1519,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$59:$A$70</c:f>
+              <c:f>[2]Hoja1!$A$59:$A$70</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1532,12 +1563,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$59:$B$70</c:f>
+              <c:f>[2]Hoja1!$B$59:$B$70</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>16.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>11</c:v>
@@ -1546,13 +1577,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60.5</c:v>
+                  <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>22.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.5</c:v>
+                  <c:v>15.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>6.5</c:v>
@@ -1561,7 +1592,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>16</c:v>
@@ -1574,24 +1605,24 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="80022528"/>
-        <c:axId val="80023936"/>
+        <c:axId val="54565504"/>
+        <c:axId val="55132544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80022528"/>
+        <c:axId val="54565504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80023936"/>
+        <c:crossAx val="55132544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80023936"/>
+        <c:axId val="55132544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1599,7 +1630,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80022528"/>
+        <c:crossAx val="54565504"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1622,7 +1653,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000167" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000167" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000178" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000178" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1645,7 +1676,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$72</c:f>
+              <c:f>[2]Hoja1!$B$72</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1656,7 +1687,7 @@
           </c:tx>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$73:$A$84</c:f>
+              <c:f>[2]Hoja1!$A$73:$A$84</c:f>
               <c:strCache>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
@@ -1700,42 +1731,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$73:$B$84</c:f>
+              <c:f>[2]Hoja1!$B$73:$B$84</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>229.5</c:v>
+                  <c:v>207.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>239.5</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>283</c:v>
+                  <c:v>260.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>101</c:v>
+                  <c:v>92.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35</c:v>
+                  <c:v>28.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>110</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>113</c:v>
+                  <c:v>97</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>2</c:v>
@@ -1745,24 +1776,24 @@
           </c:val>
         </c:ser>
         <c:gapWidth val="100"/>
-        <c:axId val="80031744"/>
-        <c:axId val="80033280"/>
+        <c:axId val="85047168"/>
+        <c:axId val="85048704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="80031744"/>
+        <c:axId val="85047168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80033280"/>
+        <c:crossAx val="85048704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80033280"/>
+        <c:axId val="85048704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1801,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="80031744"/>
+        <c:crossAx val="85047168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1793,7 +1824,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000189" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000189" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000002" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000002" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1815,7 +1846,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$2</c:f>
+              <c:f>[2]Hoja1!$B$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1830,7 +1861,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$3:$A$12</c:f>
+              <c:f>[2]Hoja1!$A$3:$A$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1868,7 +1899,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$3:$B$12</c:f>
+              <c:f>[2]Hoja1!$B$3:$B$12</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1879,16 +1910,16 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>61.5</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>9</c:v>
@@ -1900,7 +1931,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>55</c:v>
+                  <c:v>56.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1927,7 +1958,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1949,7 +1980,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Hoja1!$B$15</c:f>
+              <c:f>[2]Hoja1!$B$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1964,7 +1995,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>[1]Hoja1!$A$16:$A$25</c:f>
+              <c:f>[2]Hoja1!$A$16:$A$25</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -2002,7 +2033,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Hoja1!$B$16:$B$25</c:f>
+              <c:f>[2]Hoja1!$B$16:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -2013,16 +2044,16 @@
                   <c:v>46.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>173</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>68</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>223.5</c:v>
+                  <c:v>224</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>58.5</c:v>
@@ -2034,7 +2065,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>475.5</c:v>
+                  <c:v>477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2061,7 +2092,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2072,19 +2103,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
+      <xdr:colOff>276225</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:colOff>495300</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="1 Gráfico"/>
+        <xdr:cNvPr id="4" name="3 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2102,19 +2133,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvPr id="5" name="4 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2136,20 +2167,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="2 Gráfico"/>
+        <xdr:cNvPr id="5" name="4 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2166,20 +2197,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>219075</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvPr id="6" name="5 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2202,19 +2233,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>752475</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="3 Gráfico"/>
+        <xdr:cNvPr id="6" name="5 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2231,20 +2262,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="4 Gráfico"/>
+        <xdr:cNvPr id="7" name="6 Gráfico"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2911,6 +2942,673 @@
           </cell>
           <cell r="B83">
             <v>113</v>
+          </cell>
+        </row>
+        <row r="84">
+          <cell r="A84" t="str">
+            <v>Responsable de la Comunicación</v>
+          </cell>
+          <cell r="B84">
+            <v>2</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+      <sheetName val="Hoja2"/>
+      <sheetName val="Hoja3"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Horas realizadas semana</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="A3" t="str">
+            <v>Analisis</v>
+          </cell>
+          <cell r="B3">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="A4" t="str">
+            <v>Diseño</v>
+          </cell>
+          <cell r="B4">
+            <v>6</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>Implementación</v>
+          </cell>
+          <cell r="B5">
+            <v>35</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>Gestión de calidad</v>
+          </cell>
+          <cell r="B6">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>Gestión de configuración</v>
+          </cell>
+          <cell r="B7">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="A8" t="str">
+            <v>Gestión de proyecto</v>
+          </cell>
+          <cell r="B8">
+            <v>62</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>Verificación</v>
+          </cell>
+          <cell r="B9">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>Comunicación</v>
+          </cell>
+          <cell r="B10">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>Implantación</v>
+          </cell>
+          <cell r="B11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>Formación y entrenamiento</v>
+          </cell>
+          <cell r="B12">
+            <v>56.5</v>
+          </cell>
+        </row>
+        <row r="15">
+          <cell r="B15" t="str">
+            <v>Horas realizadas consolidado</v>
+          </cell>
+        </row>
+        <row r="16">
+          <cell r="A16" t="str">
+            <v>Analisis</v>
+          </cell>
+          <cell r="B16">
+            <v>73</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="A17" t="str">
+            <v>Diseño</v>
+          </cell>
+          <cell r="B17">
+            <v>46.5</v>
+          </cell>
+        </row>
+        <row r="18">
+          <cell r="A18" t="str">
+            <v>Implementación</v>
+          </cell>
+          <cell r="B18">
+            <v>161</v>
+          </cell>
+        </row>
+        <row r="19">
+          <cell r="A19" t="str">
+            <v>Gestión de calidad</v>
+          </cell>
+          <cell r="B19">
+            <v>79</v>
+          </cell>
+        </row>
+        <row r="20">
+          <cell r="A20" t="str">
+            <v>Gestión de configuración</v>
+          </cell>
+          <cell r="B20">
+            <v>9</v>
+          </cell>
+        </row>
+        <row r="21">
+          <cell r="A21" t="str">
+            <v>Gestión de proyecto</v>
+          </cell>
+          <cell r="B21">
+            <v>224</v>
+          </cell>
+        </row>
+        <row r="22">
+          <cell r="A22" t="str">
+            <v>Verificación</v>
+          </cell>
+          <cell r="B22">
+            <v>58.5</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="A23" t="str">
+            <v>Comunicación</v>
+          </cell>
+          <cell r="B23">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="A24" t="str">
+            <v>Implantación</v>
+          </cell>
+          <cell r="B24">
+            <v>7</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="A25" t="str">
+            <v>Formación y entrenamiento</v>
+          </cell>
+          <cell r="B25">
+            <v>477</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="B28" t="str">
+            <v>Esfuerzo estimado</v>
+          </cell>
+          <cell r="C28" t="str">
+            <v>Esfuerzo realizado</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="A30" t="str">
+            <v>Alejandro Garcia</v>
+          </cell>
+          <cell r="B30">
+            <v>15</v>
+          </cell>
+          <cell r="C30">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="A31" t="str">
+            <v>Diego Ricca</v>
+          </cell>
+          <cell r="B31">
+            <v>15</v>
+          </cell>
+          <cell r="C31">
+            <v>18.5</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="A32" t="str">
+            <v>Federico Andrade</v>
+          </cell>
+          <cell r="B32">
+            <v>15</v>
+          </cell>
+          <cell r="C32">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="A33" t="str">
+            <v>Federico Trinidad</v>
+          </cell>
+          <cell r="B33">
+            <v>15</v>
+          </cell>
+          <cell r="C33">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="A34" t="str">
+            <v>Ignacio Infante</v>
+          </cell>
+          <cell r="B34">
+            <v>15</v>
+          </cell>
+          <cell r="C34">
+            <v>14.5</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="A35" t="str">
+            <v>Javier Madeiro</v>
+          </cell>
+          <cell r="B35">
+            <v>15</v>
+          </cell>
+          <cell r="C35">
+            <v>15.5</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="A36" t="str">
+            <v>José Cordero</v>
+          </cell>
+          <cell r="B36">
+            <v>15</v>
+          </cell>
+          <cell r="C36">
+            <v>14.5</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="A37" t="str">
+            <v>Juan Ghiringhelli</v>
+          </cell>
+          <cell r="B37">
+            <v>15</v>
+          </cell>
+          <cell r="C37">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="38">
+          <cell r="A38" t="str">
+            <v>Leticia Vilariño</v>
+          </cell>
+          <cell r="B38">
+            <v>15</v>
+          </cell>
+          <cell r="C38">
+            <v>20</v>
+          </cell>
+        </row>
+        <row r="39">
+          <cell r="A39" t="str">
+            <v>Marcos Sander</v>
+          </cell>
+          <cell r="B39">
+            <v>15</v>
+          </cell>
+          <cell r="C39">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="40">
+          <cell r="A40" t="str">
+            <v>Martín Taruselli</v>
+          </cell>
+          <cell r="B40">
+            <v>15</v>
+          </cell>
+          <cell r="C40">
+            <v>14.5</v>
+          </cell>
+        </row>
+        <row r="41">
+          <cell r="A41" t="str">
+            <v>Vicente Acosta</v>
+          </cell>
+          <cell r="B41">
+            <v>15</v>
+          </cell>
+          <cell r="C41">
+            <v>12.5</v>
+          </cell>
+        </row>
+        <row r="43">
+          <cell r="B43" t="str">
+            <v>Esfuerzo estimado consolidado</v>
+          </cell>
+          <cell r="C43" t="str">
+            <v>Esfuerzo realizado consolidado</v>
+          </cell>
+        </row>
+        <row r="45">
+          <cell r="A45" t="str">
+            <v>Alejandro Garcia</v>
+          </cell>
+          <cell r="B45">
+            <v>90</v>
+          </cell>
+          <cell r="C45">
+            <v>110</v>
+          </cell>
+        </row>
+        <row r="46">
+          <cell r="A46" t="str">
+            <v>Diego Ricca</v>
+          </cell>
+          <cell r="B46">
+            <v>90</v>
+          </cell>
+          <cell r="C46">
+            <v>100</v>
+          </cell>
+        </row>
+        <row r="47">
+          <cell r="A47" t="str">
+            <v>Federico Andrade</v>
+          </cell>
+          <cell r="B47">
+            <v>90</v>
+          </cell>
+          <cell r="C47">
+            <v>104</v>
+          </cell>
+        </row>
+        <row r="48">
+          <cell r="A48" t="str">
+            <v>Federico Trinidad</v>
+          </cell>
+          <cell r="B48">
+            <v>90</v>
+          </cell>
+          <cell r="C48">
+            <v>91.5</v>
+          </cell>
+        </row>
+        <row r="49">
+          <cell r="A49" t="str">
+            <v>Ignacio Infante</v>
+          </cell>
+          <cell r="B49">
+            <v>90</v>
+          </cell>
+          <cell r="C49">
+            <v>120.5</v>
+          </cell>
+        </row>
+        <row r="50">
+          <cell r="A50" t="str">
+            <v>Javier Madeiro</v>
+          </cell>
+          <cell r="B50">
+            <v>90</v>
+          </cell>
+          <cell r="C50">
+            <v>108</v>
+          </cell>
+        </row>
+        <row r="51">
+          <cell r="A51" t="str">
+            <v>José Cordero</v>
+          </cell>
+          <cell r="B51">
+            <v>90</v>
+          </cell>
+          <cell r="C51">
+            <v>102</v>
+          </cell>
+        </row>
+        <row r="52">
+          <cell r="A52" t="str">
+            <v>Juan Ghiringhelli</v>
+          </cell>
+          <cell r="B52">
+            <v>90</v>
+          </cell>
+          <cell r="C52">
+            <v>115</v>
+          </cell>
+        </row>
+        <row r="53">
+          <cell r="A53" t="str">
+            <v>Leticia Vilariño</v>
+          </cell>
+          <cell r="B53">
+            <v>90</v>
+          </cell>
+          <cell r="C53">
+            <v>109.5</v>
+          </cell>
+        </row>
+        <row r="54">
+          <cell r="A54" t="str">
+            <v>Marcos Sander</v>
+          </cell>
+          <cell r="B54">
+            <v>90</v>
+          </cell>
+          <cell r="C54">
+            <v>93</v>
+          </cell>
+        </row>
+        <row r="55">
+          <cell r="A55" t="str">
+            <v>Martín Taruselli</v>
+          </cell>
+          <cell r="B55">
+            <v>90</v>
+          </cell>
+          <cell r="C55">
+            <v>95</v>
+          </cell>
+        </row>
+        <row r="56">
+          <cell r="A56" t="str">
+            <v>Vicente Acosta</v>
+          </cell>
+          <cell r="B56">
+            <v>90</v>
+          </cell>
+          <cell r="C56">
+            <v>88.5</v>
+          </cell>
+        </row>
+        <row r="58">
+          <cell r="B58" t="str">
+            <v xml:space="preserve">Esfuerzo realizado </v>
+          </cell>
+        </row>
+        <row r="59">
+          <cell r="A59" t="str">
+            <v>Analistas</v>
+          </cell>
+          <cell r="B59">
+            <v>16.5</v>
+          </cell>
+        </row>
+        <row r="60">
+          <cell r="A60" t="str">
+            <v>Documentador de Usuario</v>
+          </cell>
+        </row>
+        <row r="61">
+          <cell r="A61" t="str">
+            <v>Arquitecto</v>
+          </cell>
+          <cell r="B61">
+            <v>11</v>
+          </cell>
+        </row>
+        <row r="62">
+          <cell r="A62" t="str">
+            <v>Coordinador de Desarrollo</v>
+          </cell>
+          <cell r="B62">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="63">
+          <cell r="A63" t="str">
+            <v>Implementador</v>
+          </cell>
+          <cell r="B63">
+            <v>67</v>
+          </cell>
+        </row>
+        <row r="64">
+          <cell r="A64" t="str">
+            <v>Especialistas Técnicos</v>
+          </cell>
+          <cell r="B64">
+            <v>22.5</v>
+          </cell>
+        </row>
+        <row r="65">
+          <cell r="A65" t="str">
+            <v>Responsable de SQA</v>
+          </cell>
+          <cell r="B65">
+            <v>15.5</v>
+          </cell>
+        </row>
+        <row r="66">
+          <cell r="A66" t="str">
+            <v>Responsable de SCM</v>
+          </cell>
+          <cell r="B66">
+            <v>6.5</v>
+          </cell>
+        </row>
+        <row r="67">
+          <cell r="A67" t="str">
+            <v>Responsable de Verificación</v>
+          </cell>
+          <cell r="B67">
+            <v>14</v>
+          </cell>
+        </row>
+        <row r="68">
+          <cell r="A68" t="str">
+            <v>Asistente de Verificación</v>
+          </cell>
+          <cell r="B68">
+            <v>3</v>
+          </cell>
+        </row>
+        <row r="69">
+          <cell r="A69" t="str">
+            <v>Administrador</v>
+          </cell>
+          <cell r="B69">
+            <v>16</v>
+          </cell>
+        </row>
+        <row r="70">
+          <cell r="A70" t="str">
+            <v>Responsable de la Comunicación</v>
+          </cell>
+          <cell r="B70">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="72">
+          <cell r="B72" t="str">
+            <v>Esfuerzo realizado consolidado</v>
+          </cell>
+        </row>
+        <row r="73">
+          <cell r="A73" t="str">
+            <v>Analistas</v>
+          </cell>
+          <cell r="B73">
+            <v>207.5</v>
+          </cell>
+        </row>
+        <row r="74">
+          <cell r="A74" t="str">
+            <v>Documentador de Usuario</v>
+          </cell>
+          <cell r="B74">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="75">
+          <cell r="A75" t="str">
+            <v>Arquitecto</v>
+          </cell>
+          <cell r="B75">
+            <v>80</v>
+          </cell>
+        </row>
+        <row r="76">
+          <cell r="A76" t="str">
+            <v>Coordinador de Desarrollo</v>
+          </cell>
+          <cell r="B76">
+            <v>1</v>
+          </cell>
+        </row>
+        <row r="77">
+          <cell r="A77" t="str">
+            <v>Implementador</v>
+          </cell>
+          <cell r="B77">
+            <v>179</v>
+          </cell>
+        </row>
+        <row r="78">
+          <cell r="A78" t="str">
+            <v>Especialistas Técnicos</v>
+          </cell>
+          <cell r="B78">
+            <v>260.5</v>
+          </cell>
+        </row>
+        <row r="79">
+          <cell r="A79" t="str">
+            <v>Responsable de SQA</v>
+          </cell>
+          <cell r="B79">
+            <v>92.5</v>
+          </cell>
+        </row>
+        <row r="80">
+          <cell r="A80" t="str">
+            <v>Responsable de SCM</v>
+          </cell>
+          <cell r="B80">
+            <v>28.5</v>
+          </cell>
+        </row>
+        <row r="81">
+          <cell r="A81" t="str">
+            <v>Responsable de Verificación</v>
+          </cell>
+          <cell r="B81">
+            <v>96</v>
+          </cell>
+        </row>
+        <row r="82">
+          <cell r="A82" t="str">
+            <v>Asistente de Verificación</v>
+          </cell>
+          <cell r="B82">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="83">
+          <cell r="A83" t="str">
+            <v>Administrador</v>
+          </cell>
+          <cell r="B83">
+            <v>97</v>
           </cell>
         </row>
         <row r="84">
@@ -3582,7 +4280,7 @@
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B5" t="s">
         <v>92</v>
@@ -3602,19 +4300,19 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="30" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D6" s="19">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="F6" t="s">
         <v>65</v>
@@ -3628,13 +4326,13 @@
         <v>104</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="19">
         <v>4</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F7" t="s">
         <v>65</v>
@@ -3648,13 +4346,13 @@
         <v>104</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D8" s="19">
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -3665,16 +4363,16 @@
         <v>109</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D9" s="19">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F9" t="s">
         <v>65</v>
@@ -3847,7 +4545,7 @@
         <v>3.5</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
@@ -3860,7 +4558,7 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>89</v>
@@ -3872,7 +4570,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G6" t="s">
         <v>65</v>
@@ -3880,19 +4578,19 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D7" s="19">
         <v>0.5</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F7" t="s">
         <v>65</v>
@@ -3900,7 +4598,7 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>92</v>
@@ -3912,7 +4610,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -3920,7 +4618,7 @@
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>96</v>
@@ -3940,7 +4638,7 @@
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>99</v>
@@ -3960,19 +4658,19 @@
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D11" s="19">
         <v>2</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="G11" t="s">
         <v>65</v>
@@ -3980,13 +4678,13 @@
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="19">
         <v>1.5</v>
@@ -4159,13 +4857,13 @@
         <v>89</v>
       </c>
       <c r="C5" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D5" s="19">
         <v>2</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
@@ -4178,19 +4876,19 @@
     </row>
     <row r="6" spans="1:11" s="30" customFormat="1" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>89</v>
       </c>
       <c r="C6" s="29" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D6" s="19">
         <v>2</v>
       </c>
       <c r="E6" s="29" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H6" s="30" t="s">
         <v>65</v>
@@ -4198,7 +4896,7 @@
     </row>
     <row r="7" spans="1:11" s="30" customFormat="1" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>92</v>
@@ -4218,19 +4916,19 @@
     </row>
     <row r="8" spans="1:11" s="30" customFormat="1" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" s="29" t="s">
         <v>172</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>174</v>
       </c>
       <c r="D8" s="19">
         <v>2</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H8" s="30" t="s">
         <v>65</v>
@@ -4238,19 +4936,19 @@
     </row>
     <row r="9" spans="1:11" s="30" customFormat="1" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D9" s="19">
         <v>2</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F9" s="30" t="s">
         <v>65</v>
@@ -4258,10 +4956,10 @@
     </row>
     <row r="10" spans="1:11" s="30" customFormat="1" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>102</v>
@@ -4362,8 +5060,8 @@
   <sheetPr codeName="Hoja13"/>
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34:B45"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -4444,7 +5142,7 @@
       </c>
       <c r="B9" s="26">
         <f xml:space="preserve"> SUMIFS('1 _ Alejandro Garcia'!D5:'1 _ Alejandro Garcia'!D28,'1 _ Alejandro Garcia'!B5:'1 _ Alejandro Garcia'!B28,"I*") + SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!B5:'2 _ Diego Ricca'!B28,"Si") + SUMIFS('3 _ Federico Andrade'!D5:'3 _ Federico Andrade'!D28,'3 _ Federico Andrade'!B5:'3 _ Federico Andrade'!B28,"I*") + SUMIFS('4 _ Federico Trinidad'!D5:'4 _ Federico Trinidad'!D28,'4 _ Federico Trinidad'!B5:'4 _ Federico Trinidad'!B28,"I*") + SUMIFS('5 _ Ignacio Infante'!D5:'5 _ Ignacio Infante'!D28,'5 _ Ignacio Infante'!B5:'5 _ Ignacio Infante'!B28,"I*") + SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!B5:'6 _ Javier Madeiro'!B28,"I*") + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!B5:'7 _ José Cordero'!B28,"I*") + SUMIFS('8 _ Juan Ghiringhelli'!D5:'8 _ Juan Ghiringhelli'!D28,'8 _ Juan Ghiringhelli'!B5:'8 _ Juan Ghiringhelli'!B28,"I*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"I*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"I*") + SUMIFS('10 _ Marcos Sander'!D5:'10 _ Marcos Sander'!D28,'10 _ Marcos Sander'!B5:'10 _ Marcos Sander'!B28,"I*") + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!B5:'11 _ Martín Taruselli'!B28,"I*") + SUMIFS('12 _ Vicente Acosta'!D5:'12 _ Vicente Acosta'!D28,'12 _ Vicente Acosta'!B5:'12 _ Vicente Acosta'!B28,"I*")</f>
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C9" s="36"/>
     </row>
@@ -4454,7 +5152,7 @@
       </c>
       <c r="B10" s="26">
         <f xml:space="preserve"> SUMIFS('1 _ Alejandro Garcia'!D5:'1 _ Alejandro Garcia'!D28,'1 _ Alejandro Garcia'!B5:'1 _ Alejandro Garcia'!B28,"Q*") + SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!B5:'2 _ Diego Ricca'!B28,"Si") + SUMIFS('3 _ Federico Andrade'!D5:'3 _ Federico Andrade'!D28,'3 _ Federico Andrade'!B5:'3 _ Federico Andrade'!B28,"Q*") + SUMIFS('4 _ Federico Trinidad'!D5:'4 _ Federico Trinidad'!D28,'4 _ Federico Trinidad'!B5:'4 _ Federico Trinidad'!B28,"Q*") + SUMIFS('5 _ Ignacio Infante'!D5:'5 _ Ignacio Infante'!D28,'5 _ Ignacio Infante'!B5:'5 _ Ignacio Infante'!B28,"Q*") + SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!B5:'6 _ Javier Madeiro'!B28,"Q*") + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!B5:'7 _ José Cordero'!B28,"Q*") + SUMIFS('8 _ Juan Ghiringhelli'!D5:'8 _ Juan Ghiringhelli'!D28,'8 _ Juan Ghiringhelli'!B5:'8 _ Juan Ghiringhelli'!B28,"Q*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"Q*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"Q*") + SUMIFS('10 _ Marcos Sander'!D5:'10 _ Marcos Sander'!D28,'10 _ Marcos Sander'!B5:'10 _ Marcos Sander'!B28,"Q*") + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!B5:'11 _ Martín Taruselli'!B28,"Q*") + SUMIFS('12 _ Vicente Acosta'!D5:'12 _ Vicente Acosta'!D28,'12 _ Vicente Acosta'!B5:'12 _ Vicente Acosta'!B28,"Q*")</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C10" s="37"/>
     </row>
@@ -4474,7 +5172,7 @@
       </c>
       <c r="B12" s="26">
         <f xml:space="preserve"> SUMIFS('1 _ Alejandro Garcia'!D5:'1 _ Alejandro Garcia'!D28,'1 _ Alejandro Garcia'!B5:'1 _ Alejandro Garcia'!B28,"G*") + SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!B5:'2 _ Diego Ricca'!B28,"Si") + SUMIFS('3 _ Federico Andrade'!D5:'3 _ Federico Andrade'!D28,'3 _ Federico Andrade'!B5:'3 _ Federico Andrade'!B28,"G*") + SUMIFS('4 _ Federico Trinidad'!D5:'4 _ Federico Trinidad'!D28,'4 _ Federico Trinidad'!B5:'4 _ Federico Trinidad'!B28,"G*") + SUMIFS('5 _ Ignacio Infante'!D5:'5 _ Ignacio Infante'!D28,'5 _ Ignacio Infante'!B5:'5 _ Ignacio Infante'!B28,"G*") + SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!B5:'6 _ Javier Madeiro'!B28,"G*") + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!B5:'7 _ José Cordero'!B28,"G*") + SUMIFS('8 _ Juan Ghiringhelli'!D5:'8 _ Juan Ghiringhelli'!D28,'8 _ Juan Ghiringhelli'!B5:'8 _ Juan Ghiringhelli'!B28,"G*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"G*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"G*") + SUMIFS('10 _ Marcos Sander'!D5:'10 _ Marcos Sander'!D28,'10 _ Marcos Sander'!B5:'10 _ Marcos Sander'!B28,"G*") + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!B5:'11 _ Martín Taruselli'!B28,"G*") + SUMIFS('12 _ Vicente Acosta'!D5:'12 _ Vicente Acosta'!D28,'12 _ Vicente Acosta'!B5:'12 _ Vicente Acosta'!B28,"G*")</f>
-        <v>61.5</v>
+        <v>62</v>
       </c>
       <c r="C12" s="36"/>
     </row>
@@ -4514,7 +5212,7 @@
       </c>
       <c r="B16" s="27">
         <f xml:space="preserve"> SUMIFS('1 _ Alejandro Garcia'!D5:'1 _ Alejandro Garcia'!D28,'1 _ Alejandro Garcia'!B5:'1 _ Alejandro Garcia'!B28,"E*") + SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!B5:'2 _ Diego Ricca'!B28,"Si") + SUMIFS('3 _ Federico Andrade'!D5:'3 _ Federico Andrade'!D28,'3 _ Federico Andrade'!B5:'3 _ Federico Andrade'!B28,"E*") + SUMIFS('4 _ Federico Trinidad'!D5:'4 _ Federico Trinidad'!D28,'4 _ Federico Trinidad'!B5:'4 _ Federico Trinidad'!B28,"E*") + SUMIFS('5 _ Ignacio Infante'!D5:'5 _ Ignacio Infante'!D28,'5 _ Ignacio Infante'!B5:'5 _ Ignacio Infante'!B28,"E*") + SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!B5:'6 _ Javier Madeiro'!B28,"E*") + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!B5:'7 _ José Cordero'!B28,"E*") + SUMIFS('8 _ Juan Ghiringhelli'!D5:'8 _ Juan Ghiringhelli'!D28,'8 _ Juan Ghiringhelli'!B5:'8 _ Juan Ghiringhelli'!B28,"E*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"E*") + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!B5:'9 _ Leticia Vilariño'!B28,"E*") + SUMIFS('10 _ Marcos Sander'!D5:'10 _ Marcos Sander'!D28,'10 _ Marcos Sander'!B5:'10 _ Marcos Sander'!B28,"E*") + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!B5:'11 _ Martín Taruselli'!B28,"E*") + SUMIFS('12 _ Vicente Acosta'!D5:'12 _ Vicente Acosta'!D28,'12 _ Vicente Acosta'!B5:'12 _ Vicente Acosta'!B28,"E*")</f>
-        <v>55</v>
+        <v>56.5</v>
       </c>
       <c r="C16" s="9"/>
     </row>
@@ -4534,7 +5232,7 @@
       </c>
       <c r="B19" s="25">
         <f xml:space="preserve"> SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!F5:'2 _ Diego Ricca'!F28,"Si") + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!F5:'7 _ José Cordero'!F28,D5) + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!F5:'9 _ Leticia Vilariño'!F28,D5) + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!F5:'11 _ Martín Taruselli'!F28,D5)</f>
-        <v>22</v>
+        <v>16.5</v>
       </c>
       <c r="C19" s="12"/>
     </row>
@@ -4571,7 +5269,7 @@
       </c>
       <c r="B23" s="26">
         <f xml:space="preserve"> SUMIFS('2 _ Diego Ricca'!D5:'2 _ Diego Ricca'!D28,'2 _ Diego Ricca'!G5:'2 _ Diego Ricca'!G28,"Si") + SUMIFS('3 _ Federico Andrade'!D5:'3 _ Federico Andrade'!D28,'3 _ Federico Andrade'!G5:'3 _ Federico Andrade'!G28,D5) + SUMIFS('4 _ Federico Trinidad'!D5:'4 _ Federico Trinidad'!D28,'4 _ Federico Trinidad'!G5:'4 _ Federico Trinidad'!G28,D5) + SUMIFS('5 _ Ignacio Infante'!D5:'5 _ Ignacio Infante'!D28,'5 _ Ignacio Infante'!G5:'5 _ Ignacio Infante'!G28,D5) + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!G5:'7 _ José Cordero'!G28,D5) + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!H5:'9 _ Leticia Vilariño'!H28,D5) + SUMIFS('9 _ Leticia Vilariño'!D5:'9 _ Leticia Vilariño'!D28,'9 _ Leticia Vilariño'!G5:'9 _ Leticia Vilariño'!G28,D5) + SUMIFS('11 _ Martín Taruselli'!D5:'11 _ Martín Taruselli'!D28,'11 _ Martín Taruselli'!G5:'11 _ Martín Taruselli'!G28,D5) + SUMIFS('12 _ Vicente Acosta'!D5:'12 _ Vicente Acosta'!D28,'12 _ Vicente Acosta'!H5:'12 _ Vicente Acosta'!H28,D5)</f>
-        <v>60.5</v>
+        <v>67</v>
       </c>
       <c r="C23" s="12"/>
     </row>
@@ -4591,7 +5289,7 @@
       </c>
       <c r="B25" s="26">
         <f xml:space="preserve"> SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!F5:'6 _ Javier Madeiro'!F28,D5)</f>
-        <v>8.5</v>
+        <v>15.5</v>
       </c>
       <c r="C25" s="12"/>
     </row>
@@ -4621,7 +5319,7 @@
       </c>
       <c r="B28" s="26">
         <f xml:space="preserve"> SUMIFS('6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28,'6 _ Javier Madeiro'!G5:'6 _ Javier Madeiro'!G28,D5) + SUMIFS('7 _ José Cordero'!D5:'7 _ José Cordero'!D28,'7 _ José Cordero'!H5:'7 _ José Cordero'!H28,D5) + SUMIFS('8 _ Juan Ghiringhelli'!D5:'8 _ Juan Ghiringhelli'!D28,'8 _ Juan Ghiringhelli'!G5:'8 _ Juan Ghiringhelli'!G28,D5) + SUMIFS('10 _ Marcos Sander'!D5:'10 _ Marcos Sander'!D28,'10 _ Marcos Sander'!G5:'10 _ Marcos Sander'!G28,D5)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" s="12"/>
     </row>
@@ -4718,7 +5416,7 @@
       </c>
       <c r="B39" s="26">
         <f>SUM( '6 _ Javier Madeiro'!D5:'6 _ Javier Madeiro'!D28)</f>
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="C39" s="12"/>
     </row>
@@ -4810,7 +5508,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -4929,7 +5627,7 @@
     </row>
     <row r="5" spans="1:11" ht="12.75" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B5" s="28" t="s">
         <v>86</v>
@@ -4954,7 +5652,7 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="29" t="s">
         <v>89</v>
@@ -4974,7 +5672,7 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="29" t="s">
         <v>92</v>
@@ -4994,7 +5692,7 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B8" s="29" t="s">
         <v>92</v>
@@ -5014,7 +5712,7 @@
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="29" t="s">
         <v>96</v>
@@ -5034,7 +5732,7 @@
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B10" s="29" t="s">
         <v>99</v>
@@ -5054,7 +5752,7 @@
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>101</v>
@@ -5074,7 +5772,7 @@
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1">
       <c r="A12" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>104</v>
@@ -5094,7 +5792,7 @@
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B13" s="29" t="s">
         <v>99</v>
@@ -5114,7 +5812,7 @@
     </row>
     <row r="14" spans="1:11" ht="12.75" customHeight="1">
       <c r="A14" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>99</v>
@@ -5741,7 +6439,7 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>89</v>
@@ -5761,7 +6459,7 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>92</v>
@@ -5781,13 +6479,13 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D8" s="19">
         <v>1</v>
@@ -5798,7 +6496,7 @@
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>96</v>
@@ -5810,7 +6508,7 @@
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" t="s">
@@ -5819,13 +6517,13 @@
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>99</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D10" s="19">
         <v>2</v>
@@ -5834,13 +6532,13 @@
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D11" s="19">
         <v>1.5</v>
@@ -5858,7 +6556,7 @@
         <v>96</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D12" s="19">
         <v>2</v>
@@ -5947,7 +6645,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -6013,15 +6711,17 @@
         <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>89</v>
+        <v>175</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>114</v>
+        <v>176</v>
       </c>
       <c r="D5" s="19">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>5</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>177</v>
+      </c>
       <c r="F5" s="6" t="s">
         <v>65</v>
       </c>
@@ -6033,19 +6733,19 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>71</v>
+        <v>158</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>90</v>
+        <v>178</v>
       </c>
       <c r="D6" s="19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
+        <v>179</v>
       </c>
       <c r="F6" t="s">
         <v>65</v>
@@ -6053,111 +6753,90 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>73</v>
+        <v>158</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>93</v>
+        <v>138</v>
       </c>
       <c r="D7" s="19">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>115</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>116</v>
+        <v>162</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>117</v>
+        <v>180</v>
       </c>
       <c r="D8" s="19">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7"/>
-      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="F8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>118</v>
+        <v>165</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>96</v>
+        <v>119</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="D9" s="19">
-        <v>1</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="G9" t="s">
+        <v>1.5</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>99</v>
+        <v>175</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="D10" s="19">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E10" s="7"/>
+      <c r="F10" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A11" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="19">
-        <v>1.5</v>
-      </c>
+      <c r="A11" s="29"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="7"/>
-      <c r="F11" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A12" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="19">
-        <v>2</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
-      </c>
+      <c r="A12" s="29"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="30"/>
@@ -6213,7 +6892,7 @@
       </c>
       <c r="D29" s="24">
         <f>SUM(D4:D28)</f>
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12.75" customHeight="1">
@@ -6232,7 +6911,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -6301,145 +6980,101 @@
         <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>114</v>
+        <v>182</v>
       </c>
       <c r="D5" s="19">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="32"/>
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>90</v>
+        <v>138</v>
       </c>
       <c r="D6" s="19">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A7" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" s="19">
-        <v>3</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>115</v>
-      </c>
+      <c r="A7" s="29"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>117</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="19">
-        <v>1</v>
-      </c>
-      <c r="E8" s="7"/>
+        <v>3</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>184</v>
+      </c>
       <c r="G8" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>97</v>
+        <v>185</v>
       </c>
       <c r="D9" s="19">
-        <v>1</v>
+        <v>5.5</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>119</v>
+        <v>186</v>
       </c>
       <c r="G9" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A10" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D10" s="19">
-        <v>2</v>
-      </c>
+      <c r="A10" s="29"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="19"/>
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A11" s="29" t="s">
-        <v>79</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D11" s="19">
-        <v>1.5</v>
-      </c>
+      <c r="A11" s="29"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="19"/>
       <c r="E11" s="7"/>
-      <c r="F11" t="s">
-        <v>65</v>
-      </c>
     </row>
     <row r="12" spans="1:11" ht="12.75" customHeight="1">
-      <c r="A12" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D12" s="17">
-        <v>2</v>
-      </c>
-      <c r="H12" t="s">
-        <v>65</v>
-      </c>
+      <c r="A12" s="30"/>
     </row>
     <row r="13" spans="1:11" ht="12.75" customHeight="1">
       <c r="A13" s="30"/>
@@ -6582,16 +7217,16 @@
         <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D5" s="19">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>65</v>
@@ -6604,7 +7239,7 @@
     </row>
     <row r="6" spans="1:11" ht="25.5">
       <c r="A6" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>92</v>
@@ -6624,19 +7259,19 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="19">
         <v>1</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
         <v>65</v>
@@ -6644,19 +7279,19 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D8" s="19">
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F8" t="s">
         <v>65</v>
@@ -6664,19 +7299,19 @@
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D9" s="19">
         <v>2</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F9" t="s">
         <v>65</v>
@@ -6684,19 +7319,19 @@
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D10" s="19">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="F10" t="s">
         <v>65</v>
@@ -6704,10 +7339,10 @@
     </row>
     <row r="11" spans="1:11" ht="12.75" customHeight="1">
       <c r="A11" s="33" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>102</v>
@@ -6716,7 +7351,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="F11" s="34" t="s">
         <v>65</v>
@@ -6727,16 +7362,16 @@
         <v>109</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D12" s="19">
         <v>2</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="F12" t="s">
         <v>65</v>
@@ -6893,16 +7528,16 @@
         <v>68</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D5" s="19">
         <v>3</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="6" t="s">
@@ -6915,19 +7550,19 @@
     </row>
     <row r="6" spans="1:11" ht="12.75" customHeight="1">
       <c r="A6" s="29" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>76</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D6" s="19">
         <v>3</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H6" t="s">
         <v>65</v>
@@ -6935,19 +7570,19 @@
     </row>
     <row r="7" spans="1:11" ht="12.75" customHeight="1">
       <c r="A7" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D7" s="19">
         <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G7" t="s">
         <v>65</v>
@@ -6955,19 +7590,19 @@
     </row>
     <row r="8" spans="1:11" ht="12.75" customHeight="1">
       <c r="A8" s="29" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D8" s="19">
         <v>2</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G8" t="s">
         <v>65</v>
@@ -6975,19 +7610,19 @@
     </row>
     <row r="9" spans="1:11" ht="12.75" customHeight="1">
       <c r="A9" s="29" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D9" s="19">
         <v>3</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H9" t="s">
         <v>65</v>
@@ -6995,17 +7630,17 @@
     </row>
     <row r="10" spans="1:11" ht="12.75" customHeight="1">
       <c r="A10" s="29" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="19">
         <v>3</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G10" t="s">
         <v>65</v>
@@ -7016,16 +7651,16 @@
         <v>109</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D11" s="19">
         <v>3</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H11" t="s">
         <v>65</v>

</xml_diff>